<commit_message>
feat: generated lines of code metrics
</commit_message>
<xml_diff>
--- a/src/main/resources/analysis_and_metrics/presentation1/Lines of code metrics.xlsx
+++ b/src/main/resources/analysis_and_metrics/presentation1/Lines of code metrics.xlsx
@@ -452,7 +452,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,7 +591,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -599,15 +599,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -954,38 +945,62 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="19" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" xfId="31" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="22" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="4" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="25" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="16" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" xfId="29" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="6" borderId="4" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1332,7 +1347,7 @@
   <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,42 +1360,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1396,7 +1411,7 @@
       <c r="E4" s="4">
         <v>7</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>0.77780000000000005</v>
       </c>
     </row>
@@ -1416,7 +1431,7 @@
       <c r="E5" s="4">
         <v>41</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.2356</v>
       </c>
     </row>
@@ -1436,7 +1451,7 @@
       <c r="E6" s="4">
         <v>24</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>0.13789999999999999</v>
       </c>
     </row>
@@ -1456,7 +1471,7 @@
       <c r="E7" s="4">
         <v>29</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>0.16669999999999999</v>
       </c>
     </row>
@@ -1476,7 +1491,7 @@
       <c r="E8" s="4">
         <v>42</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>0.2414</v>
       </c>
     </row>
@@ -1496,7 +1511,7 @@
       <c r="E9" s="4">
         <v>29</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>0.16669999999999999</v>
       </c>
     </row>
@@ -1516,7 +1531,7 @@
       <c r="E10" s="4">
         <v>6</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>0.21429999999999999</v>
       </c>
     </row>
@@ -1536,7 +1551,7 @@
       <c r="E11" s="4">
         <v>6</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>0.21429999999999999</v>
       </c>
     </row>
@@ -1556,7 +1571,7 @@
       <c r="E12" s="4">
         <v>3</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>0.1071</v>
       </c>
     </row>
@@ -1576,7 +1591,7 @@
       <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>0.1071</v>
       </c>
     </row>
@@ -1596,7 +1611,7 @@
       <c r="E14" s="4">
         <v>3</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>0.1071</v>
       </c>
     </row>
@@ -1616,7 +1631,7 @@
       <c r="E15" s="4">
         <v>3</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>0.1071</v>
       </c>
     </row>
@@ -1636,7 +1651,7 @@
       <c r="E16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1656,7 +1671,7 @@
       <c r="E17" s="4">
         <v>3</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1676,7 +1691,7 @@
       <c r="E18" s="4">
         <v>3</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1696,7 +1711,7 @@
       <c r="E19" s="4">
         <v>3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1716,7 +1731,7 @@
       <c r="E20" s="4">
         <v>3</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1736,7 +1751,7 @@
       <c r="E21" s="4">
         <v>3</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1756,7 +1771,7 @@
       <c r="E22" s="4">
         <v>3</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1776,7 +1791,7 @@
       <c r="E23" s="4">
         <v>3</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1796,7 +1811,7 @@
       <c r="E24" s="4">
         <v>3</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1816,7 +1831,7 @@
       <c r="E25" s="4">
         <v>3</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -1836,7 +1851,7 @@
       <c r="E26" s="4">
         <v>3</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1856,7 +1871,7 @@
       <c r="E27" s="4">
         <v>3</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1876,7 +1891,7 @@
       <c r="E28" s="4">
         <v>3</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1896,7 +1911,7 @@
       <c r="E29" s="4">
         <v>3</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1916,7 +1931,7 @@
       <c r="E30" s="4">
         <v>3</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1936,7 +1951,7 @@
       <c r="E31" s="4">
         <v>3</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>0.13039999999999999</v>
       </c>
     </row>
@@ -1956,7 +1971,7 @@
       <c r="E32" s="4">
         <v>6</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>0.2727</v>
       </c>
     </row>
@@ -1976,7 +1991,7 @@
       <c r="E33" s="4">
         <v>3</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>0.13639999999999999</v>
       </c>
     </row>
@@ -1996,7 +2011,7 @@
       <c r="E34" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>0.13639999999999999</v>
       </c>
     </row>
@@ -2016,7 +2031,7 @@
       <c r="E35" s="4">
         <v>3</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>0.13639999999999999</v>
       </c>
     </row>
@@ -2036,7 +2051,7 @@
       <c r="E36" s="4">
         <v>3</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>0.13639999999999999</v>
       </c>
     </row>
@@ -2056,7 +2071,7 @@
       <c r="E37" s="4">
         <v>3</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2076,7 +2091,7 @@
       <c r="E38" s="4">
         <v>3</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2096,7 +2111,7 @@
       <c r="E39" s="4">
         <v>3</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2116,7 +2131,7 @@
       <c r="E40" s="4">
         <v>3</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2136,7 +2151,7 @@
       <c r="E41" s="4">
         <v>3</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2156,7 +2171,7 @@
       <c r="E42" s="4">
         <v>3</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2176,7 +2191,7 @@
       <c r="E43" s="4">
         <v>3</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2196,7 +2211,7 @@
       <c r="E44" s="4">
         <v>3</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2216,7 +2231,7 @@
       <c r="E45" s="4">
         <v>3</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2236,7 +2251,7 @@
       <c r="E46" s="4">
         <v>3</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="6">
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
@@ -2256,7 +2271,7 @@
       <c r="E47" s="4">
         <v>4</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <v>4.65E-2</v>
       </c>
     </row>
@@ -2276,7 +2291,7 @@
       <c r="E48" s="4">
         <v>8</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="6">
         <v>0.1047</v>
       </c>
     </row>
@@ -2296,7 +2311,7 @@
       <c r="E49" s="4">
         <v>4</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="6">
         <v>4.65E-2</v>
       </c>
     </row>
@@ -2316,7 +2331,7 @@
       <c r="E50" s="4">
         <v>14</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="6">
         <v>0.186</v>
       </c>
     </row>
@@ -2336,7 +2351,7 @@
       <c r="E51" s="4">
         <v>7</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="6">
         <v>8.14E-2</v>
       </c>
     </row>
@@ -2356,7 +2371,7 @@
       <c r="E52" s="4">
         <v>9</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="6">
         <v>0.1047</v>
       </c>
     </row>
@@ -2376,7 +2391,7 @@
       <c r="E53" s="4">
         <v>27</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="6">
         <v>0.3372</v>
       </c>
     </row>
@@ -2396,7 +2411,7 @@
       <c r="E54" s="4">
         <v>4</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="6">
         <v>5.8099999999999999E-2</v>
       </c>
     </row>
@@ -2416,7 +2431,7 @@
       <c r="E55" s="4">
         <v>16</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="6">
         <v>0.13220000000000001</v>
       </c>
     </row>
@@ -2436,7 +2451,7 @@
       <c r="E56" s="4">
         <v>4</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="6">
         <v>3.3099999999999997E-2</v>
       </c>
     </row>
@@ -2456,7 +2471,7 @@
       <c r="E57" s="4">
         <v>34</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="6">
         <v>0.28100000000000003</v>
       </c>
     </row>
@@ -2476,7 +2491,7 @@
       <c r="E58" s="4">
         <v>9</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="6">
         <v>7.4399999999999994E-2</v>
       </c>
     </row>
@@ -2496,7 +2511,7 @@
       <c r="E59" s="4">
         <v>39</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="6">
         <v>0.3306</v>
       </c>
     </row>
@@ -2516,7 +2531,7 @@
       <c r="E60" s="4">
         <v>4</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="6">
         <v>4.1300000000000003E-2</v>
       </c>
     </row>
@@ -2536,7 +2551,7 @@
       <c r="E61" s="4">
         <v>4</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="6">
         <v>3.3099999999999997E-2</v>
       </c>
     </row>
@@ -2556,7 +2571,7 @@
       <c r="E62" s="4">
         <v>4</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="6">
         <v>3.3099999999999997E-2</v>
       </c>
     </row>
@@ -2576,7 +2591,7 @@
       <c r="E63" s="4">
         <v>16</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="6">
         <v>0.1356</v>
       </c>
     </row>
@@ -2596,7 +2611,7 @@
       <c r="E64" s="4">
         <v>4</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="6">
         <v>3.39E-2</v>
       </c>
     </row>
@@ -2616,7 +2631,7 @@
       <c r="E65" s="4">
         <v>34</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="6">
         <v>0.28810000000000002</v>
       </c>
     </row>
@@ -2636,7 +2651,7 @@
       <c r="E66" s="4">
         <v>6</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="6">
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
@@ -2656,7 +2671,7 @@
       <c r="E67" s="4">
         <v>39</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="6">
         <v>0.33900000000000002</v>
       </c>
     </row>
@@ -2676,7 +2691,7 @@
       <c r="E68" s="4">
         <v>4</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="6">
         <v>4.24E-2</v>
       </c>
     </row>
@@ -2696,7 +2711,7 @@
       <c r="E69" s="4">
         <v>4</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="6">
         <v>3.39E-2</v>
       </c>
     </row>
@@ -2716,7 +2731,7 @@
       <c r="E70" s="4">
         <v>4</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="6">
         <v>3.39E-2</v>
       </c>
     </row>
@@ -2736,7 +2751,7 @@
       <c r="E71" s="4">
         <v>60</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F71" s="6">
         <v>0.85709999999999997</v>
       </c>
     </row>
@@ -2756,7 +2771,7 @@
       <c r="E72" s="4">
         <v>3</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="6">
         <v>4.2900000000000001E-2</v>
       </c>
     </row>
@@ -2776,7 +2791,7 @@
       <c r="E73" s="4">
         <v>60</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="6">
         <v>0.85709999999999997</v>
       </c>
     </row>
@@ -2796,7 +2811,7 @@
       <c r="E74" s="4">
         <v>3</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="6">
         <v>4.2900000000000001E-2</v>
       </c>
     </row>
@@ -2816,7 +2831,7 @@
       <c r="E75" s="4">
         <v>13</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="6">
         <v>0.21879999999999999</v>
       </c>
     </row>
@@ -2836,7 +2851,7 @@
       <c r="E76" s="4">
         <v>19</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F76" s="6">
         <v>0.3125</v>
       </c>
     </row>
@@ -2856,7 +2871,7 @@
       <c r="E77" s="4">
         <v>3</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="6">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
@@ -2876,7 +2891,7 @@
       <c r="E78" s="4">
         <v>18</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F78" s="6">
         <v>0.2969</v>
       </c>
     </row>
@@ -2896,7 +2911,7 @@
       <c r="E79" s="4">
         <v>11</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F79" s="6">
         <v>0.22220000000000001</v>
       </c>
     </row>
@@ -2916,7 +2931,7 @@
       <c r="E80" s="4">
         <v>17</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F80" s="6">
         <v>0.33329999999999999</v>
       </c>
     </row>
@@ -2936,7 +2951,7 @@
       <c r="E81" s="4">
         <v>3</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F81" s="6">
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
@@ -2956,7 +2971,7 @@
       <c r="E82" s="4">
         <v>13</v>
       </c>
-      <c r="F82" s="7">
+      <c r="F82" s="6">
         <v>0.25929999999999997</v>
       </c>
     </row>
@@ -2976,7 +2991,7 @@
       <c r="E83" s="4">
         <v>13</v>
       </c>
-      <c r="F83" s="7">
+      <c r="F83" s="6">
         <v>0.21879999999999999</v>
       </c>
     </row>
@@ -2996,7 +3011,7 @@
       <c r="E84" s="4">
         <v>19</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F84" s="6">
         <v>0.3125</v>
       </c>
     </row>
@@ -3016,7 +3031,7 @@
       <c r="E85" s="4">
         <v>3</v>
       </c>
-      <c r="F85" s="7">
+      <c r="F85" s="6">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
@@ -3036,7 +3051,7 @@
       <c r="E86" s="4">
         <v>18</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F86" s="6">
         <v>0.2969</v>
       </c>
     </row>
@@ -3056,7 +3071,7 @@
       <c r="E87" s="4">
         <v>33</v>
       </c>
-      <c r="F87" s="7">
+      <c r="F87" s="6">
         <v>0.76739999999999997</v>
       </c>
     </row>
@@ -3076,756 +3091,756 @@
       <c r="E88" s="4">
         <v>8</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F88" s="6">
         <v>0.186</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B91" s="4">
-        <v>0</v>
-      </c>
-      <c r="C91" s="4">
-        <v>0</v>
-      </c>
-      <c r="D91" s="4">
+      <c r="B91" s="7">
+        <v>0</v>
+      </c>
+      <c r="C91" s="7">
+        <v>0</v>
+      </c>
+      <c r="D91" s="7">
         <v>9</v>
       </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B92" s="4">
-        <v>0</v>
-      </c>
-      <c r="C92" s="4">
-        <v>0</v>
-      </c>
-      <c r="D92" s="4">
+      <c r="B92" s="7">
+        <v>0</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0</v>
+      </c>
+      <c r="D92" s="7">
         <v>174</v>
       </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B93" s="4">
-        <v>0</v>
-      </c>
-      <c r="C93" s="4">
-        <v>0</v>
-      </c>
-      <c r="D93" s="4">
+      <c r="B93" s="7">
+        <v>0</v>
+      </c>
+      <c r="C93" s="7">
+        <v>0</v>
+      </c>
+      <c r="D93" s="7">
         <v>28</v>
       </c>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B94" s="4">
-        <v>0</v>
-      </c>
-      <c r="C94" s="4">
-        <v>0</v>
-      </c>
-      <c r="D94" s="4">
+      <c r="B94" s="7">
+        <v>0</v>
+      </c>
+      <c r="C94" s="7">
+        <v>0</v>
+      </c>
+      <c r="D94" s="7">
         <v>37</v>
       </c>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="4">
-        <v>0</v>
-      </c>
-      <c r="C95" s="4">
-        <v>0</v>
-      </c>
-      <c r="D95" s="4">
+      <c r="B95" s="7">
+        <v>0</v>
+      </c>
+      <c r="C95" s="7">
+        <v>0</v>
+      </c>
+      <c r="D95" s="7">
         <v>23</v>
       </c>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="4">
-        <v>0</v>
-      </c>
-      <c r="C96" s="4">
-        <v>0</v>
-      </c>
-      <c r="D96" s="4">
+      <c r="B96" s="7">
+        <v>0</v>
+      </c>
+      <c r="C96" s="7">
+        <v>0</v>
+      </c>
+      <c r="D96" s="7">
         <v>22</v>
       </c>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B97" s="4">
-        <v>0</v>
-      </c>
-      <c r="C97" s="4">
-        <v>0</v>
-      </c>
-      <c r="D97" s="4">
+      <c r="B97" s="7">
+        <v>0</v>
+      </c>
+      <c r="C97" s="7">
+        <v>0</v>
+      </c>
+      <c r="D97" s="7">
         <v>37</v>
       </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B98" s="4">
+      <c r="B98" s="7">
         <v>6</v>
       </c>
-      <c r="C98" s="4">
-        <v>0</v>
-      </c>
-      <c r="D98" s="4">
+      <c r="C98" s="7">
+        <v>0</v>
+      </c>
+      <c r="D98" s="7">
         <v>86</v>
       </c>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B99" s="4">
+      <c r="B99" s="7">
         <v>2</v>
       </c>
-      <c r="C99" s="4">
-        <v>0</v>
-      </c>
-      <c r="D99" s="4">
+      <c r="C99" s="7">
+        <v>0</v>
+      </c>
+      <c r="D99" s="7">
         <v>121</v>
       </c>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B100" s="7">
         <v>2</v>
       </c>
-      <c r="C100" s="4">
-        <v>0</v>
-      </c>
-      <c r="D100" s="4">
+      <c r="C100" s="7">
+        <v>0</v>
+      </c>
+      <c r="D100" s="7">
         <v>118</v>
       </c>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="4">
-        <v>0</v>
-      </c>
-      <c r="C101" s="4">
-        <v>0</v>
-      </c>
-      <c r="D101" s="4">
+      <c r="B101" s="7">
+        <v>0</v>
+      </c>
+      <c r="C101" s="7">
+        <v>0</v>
+      </c>
+      <c r="D101" s="7">
         <v>70</v>
       </c>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="4">
-        <v>0</v>
-      </c>
-      <c r="C102" s="4">
-        <v>0</v>
-      </c>
-      <c r="D102" s="4">
+      <c r="B102" s="7">
+        <v>0</v>
+      </c>
+      <c r="C102" s="7">
+        <v>0</v>
+      </c>
+      <c r="D102" s="7">
         <v>70</v>
       </c>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B103" s="4">
-        <v>3</v>
-      </c>
-      <c r="C103" s="4">
-        <v>0</v>
-      </c>
-      <c r="D103" s="4">
+      <c r="B103" s="7">
+        <v>3</v>
+      </c>
+      <c r="C103" s="7">
+        <v>0</v>
+      </c>
+      <c r="D103" s="7">
         <v>64</v>
       </c>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="4">
-        <v>3</v>
-      </c>
-      <c r="C104" s="4">
-        <v>0</v>
-      </c>
-      <c r="D104" s="4">
+      <c r="B104" s="7">
+        <v>3</v>
+      </c>
+      <c r="C104" s="7">
+        <v>0</v>
+      </c>
+      <c r="D104" s="7">
         <v>54</v>
       </c>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B105" s="4">
-        <v>3</v>
-      </c>
-      <c r="C105" s="4">
-        <v>0</v>
-      </c>
-      <c r="D105" s="4">
+      <c r="B105" s="7">
+        <v>3</v>
+      </c>
+      <c r="C105" s="7">
+        <v>0</v>
+      </c>
+      <c r="D105" s="7">
         <v>64</v>
       </c>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B106" s="4">
-        <v>0</v>
-      </c>
-      <c r="C106" s="4">
-        <v>0</v>
-      </c>
-      <c r="D106" s="4">
+      <c r="B106" s="7">
+        <v>0</v>
+      </c>
+      <c r="C106" s="7">
+        <v>0</v>
+      </c>
+      <c r="D106" s="7">
         <v>43</v>
       </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G108" s="1" t="s">
+      <c r="G108" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4" t="s">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C109" s="4">
+      <c r="C109" s="9">
         <v>19</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F109" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G109" s="5">
+      <c r="G109" s="10">
         <v>1216</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C110" s="4">
+      <c r="C110" s="9">
         <v>19</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E110" s="4" t="s">
+      <c r="E110" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F110" s="4" t="s">
+      <c r="F110" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G110" s="5">
+      <c r="G110" s="10">
         <v>1113</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="9">
         <v>19</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E111" s="4" t="s">
+      <c r="E111" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F111" s="4" t="s">
+      <c r="F111" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G111" s="5">
+      <c r="G111" s="10">
         <v>1113</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B112" s="4">
-        <v>0</v>
-      </c>
-      <c r="C112" s="4">
+      <c r="B112" s="9">
+        <v>0</v>
+      </c>
+      <c r="C112" s="9">
         <v>19</v>
       </c>
-      <c r="D112" s="4">
-        <v>0</v>
-      </c>
-      <c r="E112" s="4">
-        <v>0</v>
-      </c>
-      <c r="F112" s="4">
+      <c r="D112" s="9">
+        <v>0</v>
+      </c>
+      <c r="E112" s="9">
+        <v>0</v>
+      </c>
+      <c r="F112" s="9">
         <v>11</v>
       </c>
-      <c r="G112" s="5">
+      <c r="G112" s="10">
         <v>1113</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B113" s="4">
-        <v>0</v>
-      </c>
-      <c r="C113" s="4">
-        <v>0</v>
-      </c>
-      <c r="D113" s="4">
-        <v>0</v>
-      </c>
-      <c r="E113" s="4">
-        <v>0</v>
-      </c>
-      <c r="F113" s="4">
+      <c r="B113" s="9">
+        <v>0</v>
+      </c>
+      <c r="C113" s="9">
+        <v>0</v>
+      </c>
+      <c r="D113" s="9">
+        <v>0</v>
+      </c>
+      <c r="E113" s="9">
+        <v>0</v>
+      </c>
+      <c r="F113" s="9">
         <v>190</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="9">
         <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B114" s="4">
-        <v>0</v>
-      </c>
-      <c r="C114" s="4">
+      <c r="B114" s="9">
+        <v>0</v>
+      </c>
+      <c r="C114" s="9">
         <v>10</v>
       </c>
-      <c r="D114" s="4">
-        <v>0</v>
-      </c>
-      <c r="E114" s="4">
-        <v>0</v>
-      </c>
-      <c r="F114" s="4">
+      <c r="D114" s="9">
+        <v>0</v>
+      </c>
+      <c r="E114" s="9">
+        <v>0</v>
+      </c>
+      <c r="F114" s="9">
         <v>156</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G114" s="9">
         <v>647</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B115" s="4">
-        <v>0</v>
-      </c>
-      <c r="C115" s="4">
+      <c r="B115" s="9">
+        <v>0</v>
+      </c>
+      <c r="C115" s="9">
         <v>10</v>
       </c>
-      <c r="D115" s="4">
-        <v>0</v>
-      </c>
-      <c r="E115" s="4">
-        <v>0</v>
-      </c>
-      <c r="F115" s="4">
+      <c r="D115" s="9">
+        <v>0</v>
+      </c>
+      <c r="E115" s="9">
+        <v>0</v>
+      </c>
+      <c r="F115" s="9">
         <v>341</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="9">
         <v>341</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B116" s="4">
-        <v>0</v>
-      </c>
-      <c r="C116" s="4">
-        <v>0</v>
-      </c>
-      <c r="D116" s="4">
-        <v>0</v>
-      </c>
-      <c r="E116" s="4">
-        <v>0</v>
-      </c>
-      <c r="F116" s="4">
+      <c r="B116" s="9">
+        <v>0</v>
+      </c>
+      <c r="C116" s="9">
+        <v>0</v>
+      </c>
+      <c r="D116" s="9">
+        <v>0</v>
+      </c>
+      <c r="E116" s="9">
+        <v>0</v>
+      </c>
+      <c r="F116" s="9">
         <v>150</v>
       </c>
-      <c r="G116" s="4">
+      <c r="G116" s="9">
         <v>150</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B117" s="4">
-        <v>0</v>
-      </c>
-      <c r="C117" s="4">
+      <c r="B117" s="9">
+        <v>0</v>
+      </c>
+      <c r="C117" s="9">
         <v>9</v>
       </c>
-      <c r="D117" s="4">
-        <v>0</v>
-      </c>
-      <c r="E117" s="4">
-        <v>0</v>
-      </c>
-      <c r="F117" s="4">
+      <c r="D117" s="9">
+        <v>0</v>
+      </c>
+      <c r="E117" s="9">
+        <v>0</v>
+      </c>
+      <c r="F117" s="9">
         <v>265</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G117" s="9">
         <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B118" s="4">
-        <v>0</v>
-      </c>
-      <c r="C118" s="4">
-        <v>0</v>
-      </c>
-      <c r="D118" s="4" t="s">
+      <c r="B118" s="9">
+        <v>0</v>
+      </c>
+      <c r="C118" s="9">
+        <v>0</v>
+      </c>
+      <c r="D118" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E118" s="4" t="s">
+      <c r="E118" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F118" s="4">
+      <c r="F118" s="9">
         <v>103</v>
       </c>
-      <c r="G118" s="4">
+      <c r="G118" s="9">
         <v>103</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D120" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E120" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F120" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="G120" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C121" s="12">
         <v>16</v>
       </c>
-      <c r="D121" s="4">
-        <v>0</v>
-      </c>
-      <c r="E121" s="4">
-        <v>0</v>
-      </c>
-      <c r="F121" s="4">
-        <v>0</v>
-      </c>
-      <c r="G121" s="4">
+      <c r="D121" s="12">
+        <v>0</v>
+      </c>
+      <c r="E121" s="12">
+        <v>0</v>
+      </c>
+      <c r="F121" s="12">
+        <v>0</v>
+      </c>
+      <c r="G121" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B122" s="4">
-        <v>0</v>
-      </c>
-      <c r="C122" s="4">
-        <v>0</v>
-      </c>
-      <c r="D122" s="4">
-        <v>0</v>
-      </c>
-      <c r="E122" s="5">
+      <c r="B122" s="12">
+        <v>0</v>
+      </c>
+      <c r="C122" s="12">
+        <v>0</v>
+      </c>
+      <c r="D122" s="12">
+        <v>0</v>
+      </c>
+      <c r="E122" s="13">
         <v>1113</v>
       </c>
-      <c r="F122" s="4">
-        <v>0</v>
-      </c>
-      <c r="G122" s="4">
+      <c r="F122" s="12">
+        <v>0</v>
+      </c>
+      <c r="G122" s="12">
         <v>103</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="C124" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B125" s="4">
+      <c r="B125" s="15">
         <v>75</v>
       </c>
-      <c r="C125" s="4">
+      <c r="C125" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B126" s="4">
+      <c r="B126" s="15">
         <v>70</v>
       </c>
-      <c r="C126" s="4">
+      <c r="C126" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B127" s="4">
+      <c r="B127" s="15">
         <v>16</v>
       </c>
-      <c r="C127" s="4">
+      <c r="C127" s="15">
         <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="16">
         <v>1113</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C128" s="16">
         <v>1094</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B129" s="4">
+      <c r="B129" s="15">
         <v>25</v>
       </c>
-      <c r="C129" s="4">
+      <c r="C129" s="15">
         <v>25</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B130" s="4">
+      <c r="B130" s="15">
         <v>5</v>
       </c>
-      <c r="C130" s="4">
+      <c r="C130" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B131" s="4">
+      <c r="B131" s="15">
         <v>212</v>
       </c>
-      <c r="C131" s="4">
+      <c r="C131" s="15">
         <v>212</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B132" s="4">
+      <c r="B132" s="15">
         <v>103</v>
       </c>
-      <c r="C132" s="4">
+      <c r="C132" s="15">
         <v>103</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+      <c r="A134" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="E134" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F134" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="G134" s="19" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3845,7 +3860,7 @@
       <c r="E135" s="8">
         <v>0</v>
       </c>
-      <c r="F135" s="9">
+      <c r="F135" s="18">
         <v>1113</v>
       </c>
       <c r="G135" s="8">

</xml_diff>